<commit_message>
Small update to model
</commit_message>
<xml_diff>
--- a/base_model.xlsx
+++ b/base_model.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A1AF30-2695-4D50-8DDD-33F1A551E1B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A529CD56-B4AF-48E5-836C-4D14C2778780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39405" yWindow="3585" windowWidth="21600" windowHeight="12585" xr2:uid="{325AC5AC-3898-435D-8B58-E9542B9392D3}"/>
+    <workbookView xWindow="28785" yWindow="5490" windowWidth="17925" windowHeight="11505" activeTab="1" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,23 +33,154 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Font</t>
+  </si>
+  <si>
+    <t>Arial</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Hard-coded</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Direct link</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Different file</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This Excel file is intended </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>solely for educational and informational purposes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The analysis, assumptions, and valuation contained herein represent a personal exercise in financial modeling and do </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> constitute investment advice, a recommendation to buy or sell any security, or a solicitation of any kind.</t>
+    </r>
+  </si>
+  <si>
+    <t>While efforts have been made to ensure accuracy, no representation or warranty is made as to the completeness, reliability, or accuracy of the data or calculations.</t>
+  </si>
+  <si>
+    <t>Always conduct your own research and consult with a qualified financial advisor before making any investment decisions.</t>
+  </si>
+  <si>
+    <t>Use at your own risk.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0066CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF009900"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,8 +195,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,15 +515,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1822EE-F6D2-4501-AC04-882F139B3241}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C3B520-2803-4BDC-ACDB-778D17581A2C}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="str">
+        <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,256)</f>
+        <v>Sheet1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5BED60-5D58-4477-A45E-08C960351F6B}">
+  <dimension ref="B2:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>